<commit_message>
fixed db name error
</commit_message>
<xml_diff>
--- a/91892_Support_Files/2019_appstore_games.xlsx
+++ b/91892_Support_Files/2019_appstore_games.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/stevensc9277_masseyhigh_school_nz/Documents/Old School Files/Documents/COM_201/Databases/91892_Support_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/stevensc9277_masseyhigh_school_nz/Documents/Old School Files/Documents/COM_201/Databases/L2_Databases_Apps/91892_Support_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="284" documentId="8_{A37C656A-4824-4E20-80F6-452CF8EC78C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B79C542B-F741-46FF-BA29-F193DB12F0B5}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="8_{A37C656A-4824-4E20-80F6-452CF8EC78C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB3EEAB9-1428-4B46-9AB0-A88E194E9D68}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2115" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="2805" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
@@ -5325,8 +5325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5FF0A5-369C-46D5-A0D5-3238D73BDAEA}">
   <dimension ref="A1:N244"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B233" sqref="B233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9301,7 +9301,7 @@
       <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="7" t="s">
         <v>487</v>
       </c>
       <c r="C91" t="s">
@@ -16065,8 +16065,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B91" r:id="rId1" xr:uid="{A27FB648-A698-4197-8D4D-F1B6E14B7964}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16074,7 +16077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03A7206-2C7B-4561-9225-37F25B4F1915}">
   <dimension ref="A1:Q244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>

</xml_diff>